<commit_message>
mise à jour des dossier
</commit_message>
<xml_diff>
--- a/Modèle+analyse+SEO+et+accessibilité a jour.xlsx
+++ b/Modèle+analyse+SEO+et+accessibilité a jour.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mubi\Documents\GITKRAKEN\melon78.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66B1FC4-AC1C-46CE-9B0E-CDAD79532795}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF465664-EB11-4146-83CD-753020B9C9E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20520" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="83">
   <si>
     <t>Categorie</t>
   </si>
@@ -96,9 +96,6 @@
     <t xml:space="preserve">MODIFIER LES MOTS CLES,REMPLACER LE MOT CLE PARIS PAR LYON et faire référence de manière plus ciblée à lyon. </t>
   </si>
   <si>
-    <t xml:space="preserve">DANS LE FICHIERS </t>
-  </si>
-  <si>
     <t>ACCESSIBILITE</t>
   </si>
   <si>
@@ -168,9 +165,6 @@
     <t xml:space="preserve">AJOUTER CE FICHIER A LA RACINE DU SITE POUR PERMETTRE AU ROBOTS DE EXPLORER LE SITE </t>
   </si>
   <si>
-    <t>CERTAINS IMAGES N ONT PAS UN FORMAT STANDARD</t>
-  </si>
-  <si>
     <t xml:space="preserve">IL EST PREFERABLE D UTILISER DES FORMATS DE PHOTO STANDARD POUR LE WEB </t>
   </si>
   <si>
@@ -210,9 +204,6 @@
     <t xml:space="preserve">8 CHARGEMENT DES SCRIPT JAVA à la fin </t>
   </si>
   <si>
-    <t>1 REMPLACER TOUTES LES PHOTOS QUI CONTIENNENT DU TEXTE PAR DU TEXTE, Dans la mesure du possible écrire du texte, faciliter la lecture du contenu par les robots , bon pour le référencement  ( titre 2 et titre 1)</t>
-  </si>
-  <si>
     <t>2 ADOPTER LES MOT CLES BEAUCOUP PLUS PERTINANTS EXEMPLE FAIRE REFERENCE a lyon en lieu et place de Paris + “Entreprise webdesign Lyon</t>
   </si>
   <si>
@@ -228,9 +219,6 @@
     <t xml:space="preserve">afin de ne pas être sanctionné par les robot de google ( pratique du black hat) </t>
   </si>
   <si>
-    <t xml:space="preserve">le texte du site pourra être lu par les robot de google ce qui permettra au site de remonter dans les recherches, les mettre dans des balise H1 ( tès importante pour le SEO) </t>
-  </si>
-  <si>
     <t xml:space="preserve">11 mettre du nouveau contenu régulièrement sur le site tout les 3 mois. </t>
   </si>
   <si>
@@ -271,6 +259,27 @@
   </si>
   <si>
     <t xml:space="preserve">modifier les description image , google n'apprecie pas le même description </t>
+  </si>
+  <si>
+    <t>CERTAINS IMAGES N'ONT PAS UN FORMAT STANDARD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">la description des photos doit permettre d'afficher son contenu si la photo ne se charge pas ou si l'utilisateur est mal voyante </t>
+  </si>
+  <si>
+    <t>1 REMPLACER TOUTES LES PHOTOS QUI CONTIENNENT DU TEXTE PAR DU  vrai  TEXTE, Dans la mesure du possible écrire du texte, faciliter la lecture du contenu par les robots , bon pour le référencement  ( titre 2 et titre 1)</t>
+  </si>
+  <si>
+    <t>le texte du site pourra être lu par les robot de google ce qui permettra au site de remonter dans les recherches, les mettre dans des balise H2 ( tès importante pour le SEO) , correspond exactement à la taille de caractère initiale,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">suppression des balise div avec comme contenu des mots clé invisible à l'œil nu </t>
+  </si>
+  <si>
+    <t>Black hat</t>
+  </si>
+  <si>
+    <t>Validaion w3c</t>
   </si>
 </sst>
 </file>
@@ -567,16 +576,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="41.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49" customWidth="1"/>
     <col min="3" max="3" width="31.453125" customWidth="1"/>
     <col min="4" max="4" width="43.36328125" customWidth="1"/>
     <col min="5" max="5" width="43.81640625" customWidth="1"/>
@@ -686,177 +695,173 @@
         <v>7</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="5" t="s">
+    </row>
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:26" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="B10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:26" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:26" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="6" t="s">
+      <c r="B15" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:6" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:26" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+    </row>
+    <row r="19" spans="1:6" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:6" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:6" s="6" customFormat="1" ht="108.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:6" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:6" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" t="s">
-        <v>49</v>
-      </c>
-      <c r="D24" t="s">
-        <v>50</v>
-      </c>
-      <c r="E24" t="s">
-        <v>51</v>
-      </c>
-      <c r="F24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>70</v>
-      </c>
-      <c r="B27" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>12</v>
-      </c>
-      <c r="B29" t="s">
-        <v>78</v>
-      </c>
-    </row>
+      <c r="B28" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1828,7 +1833,6 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -1837,10 +1841,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC1B391-8549-4940-AA31-9852F0C84B7A}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1852,115 +1856,128 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="45.6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:2" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>79</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mis à jour index
</commit_message>
<xml_diff>
--- a/Modèle+analyse+SEO+et+accessibilité a jour.xlsx
+++ b/Modèle+analyse+SEO+et+accessibilité a jour.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mubi\Documents\GITKRAKEN\melon78.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF465664-EB11-4146-83CD-753020B9C9E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6B1A7E-6D6A-490A-B2C6-FBA69EC16D24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="85">
   <si>
     <t>Categorie</t>
   </si>
@@ -189,18 +189,12 @@
     <t xml:space="preserve">RECOMMENDATION </t>
   </si>
   <si>
-    <t>3 EVITER LES REPETITION EXCESSIVE de mot clés</t>
-  </si>
-  <si>
     <t>5 METTRE EN PLACE UN FICHIER ROBOT;TXT</t>
   </si>
   <si>
     <t>6 CONVERTIR CERTAINES IMAGES EN FORMAT STANDARD</t>
   </si>
   <si>
-    <t>7 OPTIMISATION DU CODE HTML ET CSS</t>
-  </si>
-  <si>
     <t xml:space="preserve">8 CHARGEMENT DES SCRIPT JAVA à la fin </t>
   </si>
   <si>
@@ -222,45 +216,24 @@
     <t xml:space="preserve">11 mettre du nouveau contenu régulièrement sur le site tout les 3 mois. </t>
   </si>
   <si>
-    <t xml:space="preserve">ATTENDRE 3  ois pour faire un bilan ( puis réajustement de choix de mot clés) </t>
-  </si>
-  <si>
     <t xml:space="preserve">arriver 1er pour les mots clés </t>
   </si>
   <si>
-    <t xml:space="preserve">12 créer d'autres pages web. </t>
-  </si>
-  <si>
     <t xml:space="preserve">accessibilité </t>
   </si>
   <si>
     <t xml:space="preserve">le menu de navigation sur la page d'accueil est inaccessible </t>
   </si>
   <si>
-    <t xml:space="preserve">Modifier le positionnent du menu de navigation en pleine page </t>
-  </si>
-  <si>
-    <t>4 DONNER UN TITRE A LA PAGE WEB , POUR RENSEIGNER SUR SON CONTENU AINSI QUE LE TITRE DE LA PAGE 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">crawler ( analser on crawl ou screaming frog)  régulièrement son site , afin de repérer les optimisations à apporter </t>
   </si>
   <si>
-    <t>Chasser les contenus inutiles , afin de recnetrer l'atention des googgle bot sur le cintenus qui interesse vraiment , étudier  le trfic des pages avec GOOgle analytics</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mettre les mot clé dans des balises strong </t>
   </si>
   <si>
-    <t xml:space="preserve">optimiser les peformances ( compression / cache ) </t>
-  </si>
-  <si>
     <t xml:space="preserve">meilleures description des photos, des textes alternatifs </t>
   </si>
   <si>
-    <t xml:space="preserve">modifier les description image , google n'apprecie pas le même description </t>
-  </si>
-  <si>
     <t>CERTAINS IMAGES N'ONT PAS UN FORMAT STANDARD</t>
   </si>
   <si>
@@ -273,13 +246,46 @@
     <t>le texte du site pourra être lu par les robot de google ce qui permettra au site de remonter dans les recherches, les mettre dans des balise H2 ( tès importante pour le SEO) , correspond exactement à la taille de caractère initiale,</t>
   </si>
   <si>
-    <t xml:space="preserve">suppression des balise div avec comme contenu des mots clé invisible à l'œil nu </t>
-  </si>
-  <si>
     <t>Black hat</t>
   </si>
   <si>
-    <t>Validaion w3c</t>
+    <t>3 EVITER LES REPETITION EXCESSIVE de mot clés et les description des photos identiques</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 suppression des balise div avec comme contenu des mots clé invisible à l'œil nu , ainsi que les balises inutiles </t>
+  </si>
+  <si>
+    <t>5 DONNER UN TITRE A LA PAGE WEB , POUR RENSEIGNER SUR SON CONTENU AINSI QU' A la page 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTENDRE 3  mois pour faire un bilan ( puis réajustement de choix de mot clés) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 modifier le menu de navigation de la page 2 afin que celui-ci fonctionne correctement </t>
+  </si>
+  <si>
+    <t>Chasser les contenus inutiles , afin de recnetrer l'atention des googgle bot sur le contenus qui interesse vraiment , étudier  le trfic des pages avec GOOgle analytics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 créer d'autres pages web. </t>
+  </si>
+  <si>
+    <t>14 validation W3C</t>
+  </si>
+  <si>
+    <t>15 meilleurs description des photos et des textes alternatives</t>
+  </si>
+  <si>
+    <t xml:space="preserve">le menu de navigation de la page 2 ne fonctionne pas , et est mal positionné </t>
+  </si>
+  <si>
+    <t>7 OPTIMISATION DU CODE HTML / CSS</t>
+  </si>
+  <si>
+    <t>minimifier le code html et CSS</t>
+  </si>
+  <si>
+    <t>OK</t>
   </si>
 </sst>
 </file>
@@ -578,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -806,7 +812,7 @@
         <v>32</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>44</v>
@@ -843,10 +849,10 @@
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B26" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -855,14 +861,21 @@
         <v>12</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:6" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1841,10 +1854,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC1B391-8549-4940-AA31-9852F0C84B7A}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1854,62 +1867,103 @@
     <col min="3" max="16384" width="10.90625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="45.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:2" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>55</v>
+      <c r="C15" s="7" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1919,65 +1973,55 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>63</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
-        <v>82</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>